<commit_message>
Scottish Payroll inputsheets works sucessfully now in Automation regress Org
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite ScottishTaxGeneralAndLargeTaxcodeWeekly201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite ScottishTaxGeneralAndLargeTaxcodeWeekly201819.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Scottish Payroll InputSheet creations\Scottish Input sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F3A7F643-2925-4836-B2DE-BDA58144DBB8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="210" windowWidth="14340" windowHeight="4335" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
@@ -138,9 +139,6 @@
     <t>DONT TOUCH AUTO GLTW EMPLOYER</t>
   </si>
   <si>
-    <t>DO NOT TOUCH AUTOMATION EMP 318</t>
-  </si>
-  <si>
     <t>DO NOT TOUCH AUTOMATION EMP 319</t>
   </si>
   <si>
@@ -235,12 +233,15 @@
   </si>
   <si>
     <t>F:\\Automation_TestResults\\Payroll_Tax_NI_Directors_TestReports 201819\\201819 Scottish Payroll Net Income tax calculation Test result.xlsx</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION EMP 106</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,7 +375,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -709,7 +710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -801,11 +802,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,13 +846,13 @@
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="6">
         <v>510.64</v>
@@ -865,13 +866,13 @@
     </row>
     <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="6">
         <v>511.16</v>
@@ -885,13 +886,13 @@
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6">
         <v>2487.16</v>
@@ -905,13 +906,13 @@
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="6">
         <v>2487.6800000000003</v>
@@ -925,13 +926,13 @@
     </row>
     <row r="6" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="6">
         <v>2539.16</v>
@@ -945,13 +946,13 @@
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="6">
         <v>12627.16</v>
@@ -965,13 +966,13 @@
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="6">
         <v>12627.68</v>
@@ -985,13 +986,13 @@
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6">
         <v>12679.16</v>
@@ -1005,13 +1006,13 @@
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6">
         <v>32907.160000000003</v>
@@ -1025,13 +1026,13 @@
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="6">
         <v>32907.68</v>
@@ -1045,13 +1046,13 @@
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="6">
         <v>150479.16</v>
@@ -1065,13 +1066,13 @@
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="6">
         <v>150479.67999999999</v>
@@ -1085,13 +1086,13 @@
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="6">
         <v>10399.48</v>
@@ -1105,13 +1106,13 @@
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="6">
         <v>10399.48</v>
@@ -1125,13 +1126,13 @@
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="6">
         <v>10399.48</v>
@@ -1145,13 +1146,13 @@
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="6">
         <v>10399.48</v>
@@ -1165,10 +1166,10 @@
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>19</v>
@@ -1185,10 +1186,10 @@
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>19</v>
@@ -1205,10 +1206,10 @@
     </row>
     <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>19</v>
@@ -1225,7 +1226,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1235,11 +1236,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,10 +1302,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>17</v>
@@ -1313,13 +1314,13 @@
         <v>34</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>33</v>
@@ -1336,10 +1337,10 @@
         <v>37</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>17</v>
@@ -1348,13 +1349,13 @@
         <v>34</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>33</v>
@@ -1371,10 +1372,10 @@
         <v>37</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>17</v>
@@ -1383,13 +1384,13 @@
         <v>34</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>33</v>
@@ -1406,10 +1407,10 @@
         <v>37</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>17</v>
@@ -1418,13 +1419,13 @@
         <v>34</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>33</v>
@@ -1441,10 +1442,10 @@
         <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>17</v>
@@ -1453,13 +1454,13 @@
         <v>34</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>33</v>
@@ -1476,10 +1477,10 @@
         <v>37</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>17</v>
@@ -1488,13 +1489,13 @@
         <v>34</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>33</v>
@@ -1511,10 +1512,10 @@
         <v>37</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>17</v>
@@ -1523,13 +1524,13 @@
         <v>34</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>33</v>
@@ -1546,10 +1547,10 @@
         <v>37</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>17</v>
@@ -1558,13 +1559,13 @@
         <v>34</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>33</v>
@@ -1581,10 +1582,10 @@
         <v>37</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>17</v>
@@ -1593,13 +1594,13 @@
         <v>34</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>33</v>
@@ -1616,10 +1617,10 @@
         <v>37</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>17</v>
@@ -1628,13 +1629,13 @@
         <v>34</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>33</v>
@@ -1651,10 +1652,10 @@
         <v>37</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>17</v>
@@ -1663,13 +1664,13 @@
         <v>34</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>33</v>
@@ -1686,10 +1687,10 @@
         <v>37</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>17</v>
@@ -1698,13 +1699,13 @@
         <v>34</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>33</v>
@@ -1721,10 +1722,10 @@
         <v>37</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>17</v>
@@ -1733,13 +1734,13 @@
         <v>34</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>33</v>
@@ -1756,10 +1757,10 @@
         <v>37</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>17</v>
@@ -1768,13 +1769,13 @@
         <v>34</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>33</v>
@@ -1791,10 +1792,10 @@
         <v>37</v>
       </c>
       <c r="B16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>17</v>
@@ -1803,13 +1804,13 @@
         <v>34</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>33</v>
@@ -1826,10 +1827,10 @@
         <v>37</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>17</v>
@@ -1838,13 +1839,13 @@
         <v>34</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>33</v>
@@ -1861,10 +1862,10 @@
         <v>37</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>17</v>
@@ -1873,13 +1874,13 @@
         <v>34</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>33</v>
@@ -1896,10 +1897,10 @@
         <v>37</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>17</v>
@@ -1908,13 +1909,13 @@
         <v>34</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>33</v>
@@ -1931,10 +1932,10 @@
         <v>37</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>17</v>
@@ -1943,13 +1944,13 @@
         <v>34</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>33</v>
@@ -1963,8 +1964,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2:A13" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="A14:A20" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink ref="A2:A13" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A14:A20" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1972,7 +1973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2026,7 +2027,7 @@
         <v>31</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>2</v>
@@ -2043,10 +2044,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>17</v>
@@ -2055,13 +2056,13 @@
         <v>34</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>36</v>
@@ -2070,7 +2071,7 @@
         <v>32</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>4</v>
@@ -2078,7 +2079,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>